<commit_message>
bulk emp upload sample change
</commit_message>
<xml_diff>
--- a/assets/ebulk/employee-bulk.xlsx
+++ b/assets/ebulk/employee-bulk.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Employee ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,14 +110,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Section</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>E级</t>
-  </si>
-  <si>
-    <t>第五事业部</t>
   </si>
   <si>
     <t>软件中心</t>
@@ -521,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -537,13 +530,12 @@
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="9" max="9" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.90625" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" customWidth="1"/>
-    <col min="12" max="12" width="12" style="2" customWidth="1"/>
-    <col min="13" max="13" width="13.36328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.7265625" customWidth="1"/>
+    <col min="11" max="11" width="12" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.36328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="17.5">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="17.5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -572,19 +564,16 @@
         <v>6</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="K1" s="6" t="s">
+        <v>8</v>
+      </c>
       <c r="L1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>31632082</v>
       </c>
@@ -604,24 +593,21 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
         <v>14</v>
       </c>
+      <c r="K2" s="2">
+        <v>33688</v>
+      </c>
       <c r="L2" s="2">
-        <v>33688</v>
-      </c>
-      <c r="M2" s="2">
         <v>43335</v>
       </c>
     </row>

</xml_diff>